<commit_message>
Fixed to make an optimal solution
</commit_message>
<xml_diff>
--- a/Updated Player Data.xlsx
+++ b/Updated Player Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\OneDrive\MATLAB\Spring 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\OneDrive\MATLAB\Spring 2019\RockiesBaseball\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63F4B2A-23A9-45E5-AAC0-0F410853C3BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3EE3FF-CE0D-433E-857A-E8D2B6BA6663}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="3780" xr2:uid="{0081E226-D33A-4FEA-8237-A1A82993ED6A}"/>
   </bookViews>
@@ -1977,7 +1977,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6331,8 +6331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF8A671-CF11-4B46-9AE9-1ECBD2B152A1}">
   <dimension ref="A1:Q205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>